<commit_message>
done, added vani and josh's code
</commit_message>
<xml_diff>
--- a/beer_over_time.xlsx
+++ b/beer_over_time.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leont\Documents\Human Performance in Aerospace Environments\DICE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1DD72C-F8C4-4F4B-A262-4E43DB0255DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DB79F2-A6BE-4866-AD0F-9C94203B5C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22200" yWindow="7980" windowWidth="28800" windowHeight="15460" xr2:uid="{5B801565-1875-4445-8A33-78AFB0A4E77C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="15460" xr2:uid="{5B801565-1875-4445-8A33-78AFB0A4E77C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -74,75 +70,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -524,17 +452,17 @@
   <dimension ref="A1:K83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K83"/>
+      <selection activeCell="P15" sqref="P15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="B1">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -552,21 +480,21 @@
         <v>#N/A</v>
       </c>
       <c r="H1">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I1">
-        <v>75</v>
+        <v>960</v>
       </c>
       <c r="J1" t="e">
         <v>#N/A</v>
       </c>
       <c r="K1">
-        <v>0</v>
+        <v>900</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>975</v>
+        <v>420</v>
       </c>
       <c r="B2" t="e">
         <v>#N/A</v>
@@ -601,7 +529,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>5280</v>
+        <v>420</v>
       </c>
       <c r="B3" t="e">
         <v>#N/A</v>
@@ -636,22 +564,22 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>2625</v>
+        <v>300</v>
       </c>
       <c r="B4">
-        <v>3015</v>
+        <v>180</v>
       </c>
       <c r="C4">
-        <v>4635</v>
+        <v>180</v>
       </c>
       <c r="D4">
-        <v>750</v>
+        <v>240</v>
       </c>
       <c r="E4">
-        <v>2055</v>
+        <v>240</v>
       </c>
       <c r="F4">
-        <v>17.5</v>
+        <v>240</v>
       </c>
       <c r="G4" t="e">
         <v>#N/A</v>
@@ -666,24 +594,24 @@
         <v>#N/A</v>
       </c>
       <c r="K4">
-        <v>1050</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>1900</v>
+        <v>540</v>
       </c>
       <c r="B5">
-        <v>3187.5</v>
+        <v>600</v>
       </c>
       <c r="C5">
-        <v>2940</v>
+        <v>600</v>
       </c>
       <c r="D5">
-        <v>1670</v>
+        <v>600</v>
       </c>
       <c r="E5">
-        <v>1515</v>
+        <v>600</v>
       </c>
       <c r="F5" t="e">
         <v>#N/A</v>
@@ -698,18 +626,18 @@
         <v>#N/A</v>
       </c>
       <c r="J5">
-        <v>2940</v>
+        <v>10</v>
       </c>
       <c r="K5">
-        <v>3380</v>
+        <v>540</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>1440</v>
+        <v>630</v>
       </c>
       <c r="B6">
-        <v>1185</v>
+        <v>600</v>
       </c>
       <c r="C6" t="e">
         <v>#N/A</v>
@@ -736,12 +664,12 @@
         <v>#N/A</v>
       </c>
       <c r="K6">
-        <v>200</v>
+        <v>450</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>3580</v>
+        <v>660</v>
       </c>
       <c r="B7" t="e">
         <v>#N/A</v>
@@ -776,42 +704,42 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>780</v>
+        <v>360</v>
       </c>
       <c r="B8">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="C8" t="e">
         <v>#N/A</v>
       </c>
       <c r="D8">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="E8" t="e">
         <v>#N/A</v>
       </c>
       <c r="F8">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="G8">
-        <v>200</v>
+        <v>360</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="I8">
-        <v>720</v>
+        <v>420</v>
       </c>
       <c r="J8">
-        <v>840</v>
+        <v>240</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>325</v>
+        <v>600</v>
       </c>
       <c r="B9" t="e">
         <v>#N/A</v>
@@ -846,7 +774,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>60</v>
+        <v>720</v>
       </c>
       <c r="B10" t="e">
         <v>#N/A</v>
@@ -881,25 +809,25 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>400</v>
+        <v>540</v>
       </c>
       <c r="B11">
-        <v>637.5</v>
+        <v>480</v>
       </c>
       <c r="C11" t="e">
         <v>#N/A</v>
       </c>
       <c r="D11">
-        <v>525</v>
+        <v>600</v>
       </c>
       <c r="E11">
-        <v>562.5</v>
+        <v>960</v>
       </c>
       <c r="F11" t="e">
         <v>#N/A</v>
       </c>
       <c r="G11">
-        <v>460</v>
+        <v>600</v>
       </c>
       <c r="H11" t="e">
         <v>#N/A</v>
@@ -916,45 +844,45 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>4077.5</v>
+        <v>300</v>
       </c>
       <c r="B12">
-        <v>5565</v>
+        <v>360</v>
       </c>
       <c r="C12">
-        <v>4550</v>
+        <v>360</v>
       </c>
       <c r="D12">
-        <v>7910</v>
+        <v>360</v>
       </c>
       <c r="E12">
-        <v>4725</v>
+        <v>300</v>
       </c>
       <c r="F12">
-        <v>4550</v>
+        <v>300</v>
       </c>
       <c r="G12">
-        <v>5670</v>
+        <v>300</v>
       </c>
       <c r="H12">
-        <v>3710</v>
+        <v>300</v>
       </c>
       <c r="I12">
-        <v>5005</v>
+        <v>300</v>
       </c>
       <c r="J12">
-        <v>4270</v>
+        <v>300</v>
       </c>
       <c r="K12">
-        <v>4725</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>250</v>
+        <v>570</v>
       </c>
       <c r="B13">
-        <v>150</v>
+        <v>540</v>
       </c>
       <c r="C13" t="e">
         <v>#N/A</v>
@@ -986,7 +914,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>3447.5</v>
+        <v>270</v>
       </c>
       <c r="B14" t="e">
         <v>#N/A</v>
@@ -995,10 +923,10 @@
         <v>#N/A</v>
       </c>
       <c r="D14">
-        <v>2930</v>
+        <v>420</v>
       </c>
       <c r="E14">
-        <v>10680</v>
+        <v>360</v>
       </c>
       <c r="F14" t="e">
         <v>#N/A</v>
@@ -1016,15 +944,15 @@
         <v>#N/A</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>360</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>7080</v>
+        <v>420</v>
       </c>
       <c r="B15">
-        <v>500</v>
+        <v>480</v>
       </c>
       <c r="C15" t="e">
         <v>#N/A</v>
@@ -1056,10 +984,10 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>1860</v>
+        <v>330</v>
       </c>
       <c r="B16">
-        <v>580</v>
+        <v>300</v>
       </c>
       <c r="C16" t="e">
         <v>#N/A</v>
@@ -1071,7 +999,7 @@
         <v>#N/A</v>
       </c>
       <c r="F16">
-        <v>1425</v>
+        <v>420</v>
       </c>
       <c r="G16" t="e">
         <v>#N/A</v>
@@ -1091,77 +1019,77 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>2430</v>
+        <v>360</v>
       </c>
       <c r="B17">
-        <v>1950</v>
+        <v>300</v>
       </c>
       <c r="C17">
-        <v>3765</v>
+        <v>300</v>
       </c>
       <c r="D17">
-        <v>1890</v>
+        <v>160</v>
       </c>
       <c r="E17">
-        <v>2380</v>
+        <v>300</v>
       </c>
       <c r="F17">
-        <v>1560</v>
+        <v>300</v>
       </c>
       <c r="G17">
-        <v>1200</v>
+        <v>480</v>
       </c>
       <c r="H17" t="e">
         <v>#N/A</v>
       </c>
       <c r="I17">
-        <v>2800</v>
+        <v>480</v>
       </c>
       <c r="J17">
-        <v>2082.5</v>
+        <v>240</v>
       </c>
       <c r="K17">
-        <v>1380</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>100</v>
+        <v>540</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="D18">
-        <v>175</v>
+        <v>480</v>
       </c>
       <c r="E18">
-        <v>350</v>
+        <v>480</v>
       </c>
       <c r="F18">
-        <v>225</v>
+        <v>480</v>
       </c>
       <c r="G18">
-        <v>262.5</v>
+        <v>480</v>
       </c>
       <c r="H18">
-        <v>37.5</v>
+        <v>600</v>
       </c>
       <c r="I18">
-        <v>382.5</v>
+        <v>480</v>
       </c>
       <c r="J18">
-        <v>262.5</v>
+        <v>480</v>
       </c>
       <c r="K18">
-        <v>262.5</v>
+        <v>480</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>4650</v>
+        <v>300</v>
       </c>
       <c r="B19" t="e">
         <v>#N/A</v>
@@ -1196,34 +1124,34 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>370</v>
+        <v>540</v>
       </c>
       <c r="B20">
-        <v>640</v>
+        <v>660</v>
       </c>
       <c r="C20">
-        <v>225</v>
+        <v>540</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F20">
-        <v>25</v>
+        <v>600</v>
       </c>
       <c r="G20">
-        <v>1110</v>
+        <v>600</v>
       </c>
       <c r="H20">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I20">
-        <v>0</v>
+        <v>1080</v>
       </c>
       <c r="J20">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1231,83 +1159,83 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>8250</v>
+        <v>300</v>
       </c>
       <c r="B21">
-        <v>7290</v>
+        <v>540</v>
       </c>
       <c r="C21">
-        <v>6570</v>
+        <v>480</v>
       </c>
       <c r="D21">
-        <v>2490</v>
+        <v>540</v>
       </c>
       <c r="E21" t="e">
         <v>#N/A</v>
       </c>
       <c r="F21">
-        <v>580</v>
+        <v>720</v>
       </c>
       <c r="G21" t="e">
         <v>#N/A</v>
       </c>
       <c r="H21">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="I21" t="e">
         <v>#N/A</v>
       </c>
       <c r="J21">
-        <v>7282.5</v>
+        <v>420</v>
       </c>
       <c r="K21">
-        <v>225</v>
+        <v>900</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>2100</v>
+        <v>360</v>
       </c>
       <c r="B22">
-        <v>3060</v>
+        <v>300</v>
       </c>
       <c r="C22">
-        <v>4020</v>
+        <v>300</v>
       </c>
       <c r="D22">
-        <v>875</v>
+        <v>360</v>
       </c>
       <c r="E22">
-        <v>2625</v>
+        <v>360</v>
       </c>
       <c r="F22">
-        <v>2625</v>
+        <v>360</v>
       </c>
       <c r="G22">
-        <v>3675</v>
+        <v>300</v>
       </c>
       <c r="H22">
-        <v>1575</v>
+        <v>0</v>
       </c>
       <c r="I22">
-        <v>1580</v>
+        <v>360</v>
       </c>
       <c r="J22">
-        <v>1480</v>
+        <v>300</v>
       </c>
       <c r="K22">
-        <v>262.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>225</v>
+        <v>420</v>
       </c>
       <c r="B23">
-        <v>907.5</v>
+        <v>420</v>
       </c>
       <c r="C23">
-        <v>907.5</v>
+        <v>420</v>
       </c>
       <c r="D23" t="e">
         <v>#N/A</v>
@@ -1336,7 +1264,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>450</v>
+        <v>240</v>
       </c>
       <c r="B24" t="e">
         <v>#N/A</v>
@@ -1371,7 +1299,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>1177.5</v>
+        <v>600</v>
       </c>
       <c r="B25" t="e">
         <v>#N/A</v>
@@ -1406,19 +1334,19 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
-        <v>960</v>
+        <v>0</v>
       </c>
       <c r="B26">
-        <v>1220</v>
+        <v>600</v>
       </c>
       <c r="C26">
-        <v>615</v>
+        <v>600</v>
       </c>
       <c r="D26" t="e">
         <v>#N/A</v>
       </c>
       <c r="E26">
-        <v>525</v>
+        <v>480</v>
       </c>
       <c r="F26" t="e">
         <v>#N/A</v>
@@ -1441,7 +1369,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
-        <v>1410</v>
+        <v>720</v>
       </c>
       <c r="B27" t="e">
         <v>#N/A</v>
@@ -1456,7 +1384,7 @@
         <v>#N/A</v>
       </c>
       <c r="F27">
-        <v>300</v>
+        <v>720</v>
       </c>
       <c r="G27" t="e">
         <v>#N/A</v>
@@ -1476,10 +1404,10 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B28">
-        <v>1100</v>
+        <v>480</v>
       </c>
       <c r="C28" t="e">
         <v>#N/A</v>
@@ -1491,19 +1419,19 @@
         <v>#N/A</v>
       </c>
       <c r="F28">
-        <v>2050</v>
+        <v>240</v>
       </c>
       <c r="G28">
-        <v>1660</v>
+        <v>300</v>
       </c>
       <c r="H28">
-        <v>677.5</v>
+        <v>360</v>
       </c>
       <c r="I28">
-        <v>1282.5</v>
+        <v>180</v>
       </c>
       <c r="J28">
-        <v>1035</v>
+        <v>360</v>
       </c>
       <c r="K28" t="e">
         <v>#N/A</v>
@@ -1511,10 +1439,10 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
-        <v>1185</v>
+        <v>720</v>
       </c>
       <c r="B29">
-        <v>1057.5</v>
+        <v>720</v>
       </c>
       <c r="C29" t="e">
         <v>#N/A</v>
@@ -1546,7 +1474,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
-        <v>0</v>
+        <v>1200</v>
       </c>
       <c r="B30" t="e">
         <v>#N/A</v>
@@ -1581,7 +1509,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
-        <v>2220</v>
+        <v>240</v>
       </c>
       <c r="B31" t="e">
         <v>#N/A</v>
@@ -1616,7 +1544,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>3450</v>
+        <v>180</v>
       </c>
       <c r="B32" t="e">
         <v>#N/A</v>
@@ -1628,7 +1556,7 @@
         <v>#N/A</v>
       </c>
       <c r="E32">
-        <v>2250</v>
+        <v>300</v>
       </c>
       <c r="F32" t="e">
         <v>#N/A</v>
@@ -1651,10 +1579,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
-        <v>4210</v>
+        <v>420</v>
       </c>
       <c r="B33">
-        <v>3255</v>
+        <v>300</v>
       </c>
       <c r="C33" t="e">
         <v>#N/A</v>
@@ -1663,22 +1591,22 @@
         <v>#N/A</v>
       </c>
       <c r="E33">
-        <v>2540</v>
+        <v>360</v>
       </c>
       <c r="F33">
-        <v>3622.5</v>
+        <v>360</v>
       </c>
       <c r="G33" t="e">
         <v>#N/A</v>
       </c>
       <c r="H33">
-        <v>1815</v>
+        <v>300</v>
       </c>
       <c r="I33" t="e">
         <v>#N/A</v>
       </c>
       <c r="J33">
-        <v>3255</v>
+        <v>300</v>
       </c>
       <c r="K33" t="e">
         <v>#N/A</v>
@@ -1686,7 +1614,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
-        <v>2490</v>
+        <v>420</v>
       </c>
       <c r="B34" t="e">
         <v>#N/A</v>
@@ -1721,77 +1649,77 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
-        <v>0</v>
+        <v>780</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="D35">
-        <v>75</v>
+        <v>660</v>
       </c>
       <c r="E35">
-        <v>210</v>
+        <v>600</v>
       </c>
       <c r="F35">
-        <v>37.5</v>
+        <v>660</v>
       </c>
       <c r="G35">
-        <v>75</v>
+        <v>720</v>
       </c>
       <c r="H35">
-        <v>150</v>
+        <v>720</v>
       </c>
       <c r="I35">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="J35">
-        <v>1477.5</v>
+        <v>840</v>
       </c>
       <c r="K35">
-        <v>75</v>
+        <v>720</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
-        <v>7125</v>
+        <v>450</v>
       </c>
       <c r="B36">
-        <v>3950</v>
+        <v>480</v>
       </c>
       <c r="C36">
-        <v>3950</v>
+        <v>480</v>
       </c>
       <c r="D36">
-        <v>6285</v>
+        <v>480</v>
       </c>
       <c r="E36">
-        <v>5390</v>
+        <v>480</v>
       </c>
       <c r="F36" t="e">
         <v>#N/A</v>
       </c>
       <c r="G36">
-        <v>2925</v>
+        <v>480</v>
       </c>
       <c r="H36" t="e">
         <v>#N/A</v>
       </c>
       <c r="I36">
-        <v>533.5</v>
+        <v>330</v>
       </c>
       <c r="J36" t="e">
         <v>#N/A</v>
       </c>
       <c r="K36">
-        <v>4845</v>
+        <v>480</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
-        <v>580</v>
+        <v>660</v>
       </c>
       <c r="B37" t="e">
         <v>#N/A</v>
@@ -1826,7 +1754,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>3360</v>
+        <v>780</v>
       </c>
       <c r="B38" t="e">
         <v>#N/A</v>
@@ -1838,19 +1766,19 @@
         <v>#N/A</v>
       </c>
       <c r="E38">
-        <v>1155</v>
+        <v>720</v>
       </c>
       <c r="F38" t="e">
         <v>#N/A</v>
       </c>
       <c r="G38">
-        <v>2210</v>
+        <v>780</v>
       </c>
       <c r="H38" t="e">
         <v>#N/A</v>
       </c>
       <c r="I38">
-        <v>1800</v>
+        <v>720</v>
       </c>
       <c r="J38" t="e">
         <v>#N/A</v>
@@ -1861,7 +1789,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
-        <v>1050</v>
+        <v>600</v>
       </c>
       <c r="B39" t="e">
         <v>#N/A</v>
@@ -1870,7 +1798,7 @@
         <v>#N/A</v>
       </c>
       <c r="D39">
-        <v>787.5</v>
+        <v>480</v>
       </c>
       <c r="E39" t="e">
         <v>#N/A</v>
@@ -1885,7 +1813,7 @@
         <v>#N/A</v>
       </c>
       <c r="I39">
-        <v>1290</v>
+        <v>480</v>
       </c>
       <c r="J39" t="e">
         <v>#N/A</v>
@@ -1896,7 +1824,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
-        <v>2310</v>
+        <v>420</v>
       </c>
       <c r="B40" t="e">
         <v>#N/A</v>
@@ -1908,16 +1836,16 @@
         <v>#N/A</v>
       </c>
       <c r="E40">
-        <v>4455</v>
+        <v>240</v>
       </c>
       <c r="F40">
-        <v>3495</v>
+        <v>240</v>
       </c>
       <c r="G40" t="e">
         <v>#N/A</v>
       </c>
       <c r="H40">
-        <v>1225</v>
+        <v>240</v>
       </c>
       <c r="I40" t="e">
         <v>#N/A</v>
@@ -1931,7 +1859,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
-        <v>525</v>
+        <v>600</v>
       </c>
       <c r="B41" t="e">
         <v>#N/A</v>
@@ -1966,10 +1894,10 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
-        <v>187.5</v>
+        <v>600</v>
       </c>
       <c r="B42">
-        <v>187.5</v>
+        <v>600</v>
       </c>
       <c r="C42" t="e">
         <v>#N/A</v>
@@ -2001,42 +1929,42 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>650</v>
+        <v>480</v>
       </c>
       <c r="B43">
-        <v>650</v>
+        <v>360</v>
       </c>
       <c r="C43" t="e">
         <v>#N/A</v>
       </c>
       <c r="D43">
-        <v>130</v>
+        <v>480</v>
       </c>
       <c r="E43">
-        <v>877.5</v>
+        <v>300</v>
       </c>
       <c r="F43">
-        <v>225</v>
+        <v>360</v>
       </c>
       <c r="G43">
-        <v>130</v>
+        <v>480</v>
       </c>
       <c r="H43">
-        <v>450</v>
+        <v>480</v>
       </c>
       <c r="I43">
         <v>0</v>
       </c>
       <c r="J43">
-        <v>50</v>
+        <v>300</v>
       </c>
       <c r="K43">
-        <v>75</v>
+        <v>300</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
-        <v>802.5</v>
+        <v>600</v>
       </c>
       <c r="B44" t="e">
         <v>#N/A</v>
@@ -2048,13 +1976,13 @@
         <v>#N/A</v>
       </c>
       <c r="E44">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="F44" t="e">
         <v>#N/A</v>
       </c>
       <c r="G44">
-        <v>675</v>
+        <v>480</v>
       </c>
       <c r="H44" t="e">
         <v>#N/A</v>
@@ -2066,12 +1994,12 @@
         <v>#N/A</v>
       </c>
       <c r="K44">
-        <v>562.5</v>
+        <v>720</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
-        <v>1680</v>
+        <v>240</v>
       </c>
       <c r="B45" t="e">
         <v>#N/A</v>
@@ -2080,10 +2008,10 @@
         <v>#N/A</v>
       </c>
       <c r="D45">
-        <v>4320</v>
+        <v>960</v>
       </c>
       <c r="E45">
-        <v>3030</v>
+        <v>240</v>
       </c>
       <c r="F45" t="e">
         <v>#N/A</v>
@@ -2095,27 +2023,27 @@
         <v>#N/A</v>
       </c>
       <c r="I45">
-        <v>2880</v>
+        <v>480</v>
       </c>
       <c r="J45">
-        <v>0</v>
+        <v>240</v>
       </c>
       <c r="K45">
-        <v>84</v>
+        <v>720</v>
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
-        <v>8</v>
+        <v>900</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="C46" t="e">
         <v>#N/A</v>
       </c>
       <c r="D46">
-        <v>1680</v>
+        <v>660</v>
       </c>
       <c r="E46" t="e">
         <v>#N/A</v>
@@ -2141,22 +2069,22 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
-        <v>2055</v>
+        <v>390</v>
       </c>
       <c r="B47">
-        <v>1815</v>
+        <v>390</v>
       </c>
       <c r="C47">
-        <v>2055</v>
+        <v>420</v>
       </c>
       <c r="D47">
-        <v>3735</v>
+        <v>390</v>
       </c>
       <c r="E47">
-        <v>3450</v>
+        <v>360</v>
       </c>
       <c r="F47">
-        <v>3975</v>
+        <v>480</v>
       </c>
       <c r="G47" t="e">
         <v>#N/A</v>
@@ -2165,18 +2093,18 @@
         <v>#N/A</v>
       </c>
       <c r="I47">
-        <v>4170</v>
+        <v>360</v>
       </c>
       <c r="J47">
-        <v>4650</v>
+        <v>420</v>
       </c>
       <c r="K47">
-        <v>2887.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
-        <v>0</v>
+        <v>360</v>
       </c>
       <c r="B48" t="e">
         <v>#N/A</v>
@@ -2211,7 +2139,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
-        <v>885</v>
+        <v>720</v>
       </c>
       <c r="B49" t="e">
         <v>#N/A</v>
@@ -2220,7 +2148,7 @@
         <v>#N/A</v>
       </c>
       <c r="D49">
-        <v>970</v>
+        <v>300</v>
       </c>
       <c r="E49" t="e">
         <v>#N/A</v>
@@ -2246,7 +2174,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
-        <v>3885</v>
+        <v>660</v>
       </c>
       <c r="B50" t="e">
         <v>#N/A</v>
@@ -2281,34 +2209,34 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="B51">
-        <v>490</v>
+        <v>420</v>
       </c>
       <c r="C51" t="e">
         <v>#N/A</v>
       </c>
       <c r="D51">
-        <v>90</v>
+        <v>600</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="F51">
-        <v>75</v>
+        <v>600</v>
       </c>
       <c r="G51" t="e">
         <v>#N/A</v>
       </c>
       <c r="H51">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="I51">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="J51">
-        <v>630</v>
+        <v>600</v>
       </c>
       <c r="K51" t="e">
         <v>#N/A</v>
@@ -2316,7 +2244,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
-        <v>7550</v>
+        <v>240</v>
       </c>
       <c r="B52" t="e">
         <v>#N/A</v>
@@ -2334,7 +2262,7 @@
         <v>#N/A</v>
       </c>
       <c r="G52">
-        <v>560</v>
+        <v>160</v>
       </c>
       <c r="H52" t="e">
         <v>#N/A</v>
@@ -2351,7 +2279,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>750</v>
+        <v>600</v>
       </c>
       <c r="B53" t="e">
         <v>#N/A</v>
@@ -2360,7 +2288,7 @@
         <v>#N/A</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="E53" t="e">
         <v>#N/A</v>
@@ -2369,7 +2297,7 @@
         <v>#N/A</v>
       </c>
       <c r="G53">
-        <v>150</v>
+        <v>540</v>
       </c>
       <c r="H53" t="e">
         <v>#N/A</v>
@@ -2386,7 +2314,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
-        <v>2325</v>
+        <v>540</v>
       </c>
       <c r="B54" t="e">
         <v>#N/A</v>
@@ -2421,7 +2349,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
-        <v>100</v>
+        <v>720</v>
       </c>
       <c r="B55" t="e">
         <v>#N/A</v>
@@ -2439,13 +2367,13 @@
         <v>#N/A</v>
       </c>
       <c r="G55">
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="H55">
         <v>0</v>
       </c>
       <c r="I55">
-        <v>150</v>
+        <v>600</v>
       </c>
       <c r="J55" t="e">
         <v>#N/A</v>
@@ -2456,7 +2384,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
-        <v>1050</v>
+        <v>480</v>
       </c>
       <c r="B56" t="e">
         <v>#N/A</v>
@@ -2491,34 +2419,34 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
-        <v>525</v>
+        <v>720</v>
       </c>
       <c r="B57">
-        <v>525</v>
+        <v>720</v>
       </c>
       <c r="C57">
-        <v>855</v>
+        <v>900</v>
       </c>
       <c r="D57" t="e">
         <v>#N/A</v>
       </c>
       <c r="E57">
-        <v>300</v>
+        <v>720</v>
       </c>
       <c r="F57">
-        <v>225</v>
+        <v>600</v>
       </c>
       <c r="G57" t="e">
         <v>#N/A</v>
       </c>
       <c r="H57">
-        <v>225</v>
+        <v>720</v>
       </c>
       <c r="I57" t="e">
         <v>#N/A</v>
       </c>
       <c r="J57">
-        <v>375</v>
+        <v>720</v>
       </c>
       <c r="K57" t="e">
         <v>#N/A</v>
@@ -2526,7 +2454,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="B58" t="e">
         <v>#N/A</v>
@@ -2538,7 +2466,7 @@
         <v>#N/A</v>
       </c>
       <c r="E58">
-        <v>3375</v>
+        <v>360</v>
       </c>
       <c r="F58" t="e">
         <v>#N/A</v>
@@ -2561,13 +2489,13 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
-        <v>9000</v>
+        <v>120</v>
       </c>
       <c r="B59">
-        <v>2775</v>
+        <v>60</v>
       </c>
       <c r="C59">
-        <v>3720</v>
+        <v>120</v>
       </c>
       <c r="D59" t="e">
         <v>#N/A</v>
@@ -2576,7 +2504,7 @@
         <v>#N/A</v>
       </c>
       <c r="F59">
-        <v>3045</v>
+        <v>60</v>
       </c>
       <c r="G59" t="e">
         <v>#N/A</v>
@@ -2588,15 +2516,15 @@
         <v>#N/A</v>
       </c>
       <c r="J59">
-        <v>3390</v>
+        <v>45</v>
       </c>
       <c r="K59">
-        <v>3630</v>
+        <v>45</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
-        <v>2100</v>
+        <v>180</v>
       </c>
       <c r="B60" t="e">
         <v>#N/A</v>
@@ -2614,10 +2542,10 @@
         <v>#N/A</v>
       </c>
       <c r="G60">
-        <v>2100</v>
+        <v>240</v>
       </c>
       <c r="H60">
-        <v>315</v>
+        <v>360</v>
       </c>
       <c r="I60" t="e">
         <v>#N/A</v>
@@ -2631,7 +2559,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
-        <v>175</v>
+        <v>240</v>
       </c>
       <c r="B61" t="e">
         <v>#N/A</v>
@@ -2666,42 +2594,42 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
-        <v>525</v>
+        <v>480</v>
       </c>
       <c r="B62">
-        <v>477.5</v>
+        <v>360</v>
       </c>
       <c r="C62">
-        <v>525</v>
+        <v>300</v>
       </c>
       <c r="D62">
-        <v>997.5</v>
+        <v>360</v>
       </c>
       <c r="E62">
-        <v>825</v>
+        <v>420</v>
       </c>
       <c r="F62">
-        <v>437.5</v>
+        <v>48</v>
       </c>
       <c r="G62">
-        <v>677.5</v>
+        <v>300</v>
       </c>
       <c r="H62">
-        <v>1050</v>
+        <v>240</v>
       </c>
       <c r="I62">
-        <v>810</v>
+        <v>540</v>
       </c>
       <c r="J62">
-        <v>1125</v>
+        <v>480</v>
       </c>
       <c r="K62">
-        <v>1125</v>
+        <v>420</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
-        <v>750</v>
+        <v>720</v>
       </c>
       <c r="B63" t="e">
         <v>#N/A</v>
@@ -2716,7 +2644,7 @@
         <v>#N/A</v>
       </c>
       <c r="F63">
-        <v>2490</v>
+        <v>600</v>
       </c>
       <c r="G63" t="e">
         <v>#N/A</v>
@@ -2725,7 +2653,7 @@
         <v>#N/A</v>
       </c>
       <c r="I63">
-        <v>3210</v>
+        <v>600</v>
       </c>
       <c r="J63" t="e">
         <v>#N/A</v>
@@ -2736,22 +2664,22 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
-        <v>75</v>
+        <v>480</v>
       </c>
       <c r="B64">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>540</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>480</v>
       </c>
       <c r="G64" t="e">
         <v>#N/A</v>
@@ -2771,7 +2699,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
-        <v>787.5</v>
+        <v>240</v>
       </c>
       <c r="B65" t="e">
         <v>#N/A</v>
@@ -2780,7 +2708,7 @@
         <v>#N/A</v>
       </c>
       <c r="D65">
-        <v>750</v>
+        <v>360</v>
       </c>
       <c r="E65" t="e">
         <v>#N/A</v>
@@ -2789,7 +2717,7 @@
         <v>#N/A</v>
       </c>
       <c r="G65">
-        <v>787.5</v>
+        <v>540</v>
       </c>
       <c r="H65" t="e">
         <v>#N/A</v>
@@ -2806,7 +2734,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>1380</v>
+        <v>540</v>
       </c>
       <c r="B66" t="e">
         <v>#N/A</v>
@@ -2815,36 +2743,36 @@
         <v>#N/A</v>
       </c>
       <c r="D66">
-        <v>150</v>
+        <v>720</v>
       </c>
       <c r="E66">
-        <v>1170</v>
+        <v>600</v>
       </c>
       <c r="F66">
-        <v>200</v>
+        <v>540</v>
       </c>
       <c r="G66" t="e">
         <v>#N/A</v>
       </c>
       <c r="H66">
-        <v>1507.5</v>
+        <v>480</v>
       </c>
       <c r="I66">
-        <v>337.5</v>
+        <v>480</v>
       </c>
       <c r="J66" t="e">
         <v>#N/A</v>
       </c>
       <c r="K66">
-        <v>262.5</v>
+        <v>600</v>
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
-        <v>1590</v>
+        <v>480</v>
       </c>
       <c r="B67">
-        <v>1665</v>
+        <v>360</v>
       </c>
       <c r="C67" t="e">
         <v>#N/A</v>
@@ -2876,7 +2804,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
-        <v>345</v>
+        <v>540</v>
       </c>
       <c r="B68" t="e">
         <v>#N/A</v>
@@ -2911,10 +2839,10 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
-        <v>570</v>
+        <v>550</v>
       </c>
       <c r="B69">
-        <v>225</v>
+        <v>540</v>
       </c>
       <c r="C69" t="e">
         <v>#N/A</v>
@@ -2941,12 +2869,12 @@
         <v>#N/A</v>
       </c>
       <c r="K69">
-        <v>337.5</v>
+        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
-        <v>1200</v>
+        <v>480</v>
       </c>
       <c r="B70" t="e">
         <v>#N/A</v>
@@ -2981,28 +2909,28 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
-        <v>240</v>
+        <v>720</v>
       </c>
       <c r="B71">
+        <v>720</v>
+      </c>
+      <c r="C71">
+        <v>720</v>
+      </c>
+      <c r="D71">
         <v>360</v>
       </c>
-      <c r="C71">
-        <v>240</v>
-      </c>
-      <c r="D71">
-        <v>3787.5</v>
-      </c>
       <c r="E71" t="e">
         <v>#N/A</v>
       </c>
       <c r="F71">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="G71" t="e">
         <v>#N/A</v>
       </c>
       <c r="H71">
-        <v>1140</v>
+        <v>420</v>
       </c>
       <c r="I71" t="e">
         <v>#N/A</v>
@@ -3016,16 +2944,16 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="B72">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="C72">
         <v>0</v>
       </c>
       <c r="D72">
-        <v>3435</v>
+        <v>660</v>
       </c>
       <c r="E72" t="e">
         <v>#N/A</v>
@@ -3040,21 +2968,21 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <v>0</v>
+        <v>960</v>
       </c>
       <c r="J72" t="e">
         <v>#N/A</v>
       </c>
       <c r="K72">
-        <v>175</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>4455</v>
+        <v>720</v>
       </c>
       <c r="B73">
-        <v>4500</v>
+        <v>600</v>
       </c>
       <c r="C73" t="e">
         <v>#N/A</v>
@@ -3086,19 +3014,19 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="B74">
         <v>0</v>
       </c>
       <c r="C74">
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>720</v>
       </c>
       <c r="F74" t="e">
         <v>#N/A</v>
@@ -3121,7 +3049,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
-        <v>787.5</v>
+        <v>240</v>
       </c>
       <c r="B75" t="e">
         <v>#N/A</v>
@@ -3130,33 +3058,33 @@
         <v>#N/A</v>
       </c>
       <c r="D75">
-        <v>735</v>
+        <v>240</v>
       </c>
       <c r="E75">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="F75">
-        <v>4455</v>
+        <v>240</v>
       </c>
       <c r="G75">
-        <v>375</v>
+        <v>540</v>
       </c>
       <c r="H75">
-        <v>525</v>
+        <v>240</v>
       </c>
       <c r="I75">
-        <v>2662.5</v>
+        <v>300</v>
       </c>
       <c r="J75">
-        <v>2220</v>
+        <v>180</v>
       </c>
       <c r="K75">
-        <v>645</v>
+        <v>180</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="B76" t="e">
         <v>#N/A</v>
@@ -3191,7 +3119,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
-        <v>3160</v>
+        <v>360</v>
       </c>
       <c r="B77" t="e">
         <v>#N/A</v>
@@ -3226,10 +3154,10 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78">
-        <v>675</v>
+        <v>720</v>
       </c>
       <c r="B78">
-        <v>490</v>
+        <v>900</v>
       </c>
       <c r="C78" t="e">
         <v>#N/A</v>
@@ -3241,7 +3169,7 @@
         <v>#N/A</v>
       </c>
       <c r="F78">
-        <v>1575</v>
+        <v>300</v>
       </c>
       <c r="G78" t="e">
         <v>#N/A</v>
@@ -3261,34 +3189,34 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79">
-        <v>0</v>
+        <v>1420</v>
       </c>
       <c r="B79">
-        <v>4770</v>
+        <v>720</v>
       </c>
       <c r="C79">
-        <v>1920</v>
+        <v>780</v>
       </c>
       <c r="D79">
-        <v>4320</v>
+        <v>480</v>
       </c>
       <c r="E79">
-        <v>2550</v>
+        <v>720</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>840</v>
       </c>
       <c r="G79">
-        <v>1050</v>
+        <v>780</v>
       </c>
       <c r="H79">
-        <v>2670</v>
+        <v>480</v>
       </c>
       <c r="I79" t="e">
         <v>#N/A</v>
       </c>
       <c r="J79">
-        <v>142.5</v>
+        <v>720</v>
       </c>
       <c r="K79" t="e">
         <v>#N/A</v>
@@ -3296,7 +3224,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80">
-        <v>885</v>
+        <v>360</v>
       </c>
       <c r="B80" t="e">
         <v>#N/A</v>
@@ -3305,7 +3233,7 @@
         <v>#N/A</v>
       </c>
       <c r="D80">
-        <v>760</v>
+        <v>480</v>
       </c>
       <c r="E80" t="e">
         <v>#N/A</v>
@@ -3331,7 +3259,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81">
-        <v>1635</v>
+        <v>600</v>
       </c>
       <c r="B81" t="e">
         <v>#N/A</v>
@@ -3366,7 +3294,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82">
-        <v>375</v>
+        <v>600</v>
       </c>
       <c r="B82" t="e">
         <v>#N/A</v>
@@ -3375,7 +3303,7 @@
         <v>#N/A</v>
       </c>
       <c r="D82">
-        <v>437.5</v>
+        <v>360</v>
       </c>
       <c r="E82" t="e">
         <v>#N/A</v>
@@ -3401,19 +3329,19 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83">
-        <v>1300</v>
+        <v>600</v>
       </c>
       <c r="B83">
-        <v>2690</v>
+        <v>600</v>
       </c>
       <c r="C83">
-        <v>2475</v>
+        <v>600</v>
       </c>
       <c r="D83">
-        <v>2662.5</v>
+        <v>540</v>
       </c>
       <c r="E83">
-        <v>3350</v>
+        <v>300</v>
       </c>
       <c r="F83" t="e">
         <v>#N/A</v>
@@ -3451,6 +3379,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010090E4CF1CF3D2E44C9EBC5F33876394C9" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="201bc20606f8f56f1c181d731efb1b69">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="28e706f3083a55b82f61ab241e6ec084">
     <xsd:element name="properties">
@@ -3564,15 +3501,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3580,6 +3508,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B0049AF-8F97-4289-8FC2-C5BF8A2A5BBC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C664BE2-481D-4013-B3DA-4E6614716BCA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3591,14 +3527,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B0049AF-8F97-4289-8FC2-C5BF8A2A5BBC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>